<commit_message>
Testes com fundo complexo
</commit_message>
<xml_diff>
--- a/testes.xlsx
+++ b/testes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chan\AndroidStudioProjects\TTS-OCR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="209">
   <si>
     <t>AMBIENTE</t>
   </si>
@@ -618,6 +618,39 @@
   </si>
   <si>
     <t>In Lhepmmcm nu m u m m hes! Lhvnguf nh n m min, -mt cncm n mmm; whole and mum m shanerand dealmy n n not so good</t>
+  </si>
+  <si>
+    <t>wsmw</t>
+  </si>
+  <si>
+    <t>Mmemum fawccn</t>
+  </si>
+  <si>
+    <t>Millenium falcon</t>
+  </si>
+  <si>
+    <t>BATMAN</t>
+  </si>
+  <si>
+    <t>The Joker</t>
+  </si>
+  <si>
+    <t>Gothan City</t>
+  </si>
+  <si>
+    <t>Gothan Citn</t>
+  </si>
+  <si>
+    <t>The Penguin</t>
+  </si>
+  <si>
+    <t>The Tenguin</t>
+  </si>
+  <si>
+    <t>Ji</t>
+  </si>
+  <si>
+    <t>Milleniuh 15can</t>
   </si>
 </sst>
 </file>
@@ -863,6 +896,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -896,8 +931,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1178,10 +1211,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N133"/>
+  <dimension ref="A1:N144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L132" sqref="L132"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,30 +1236,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J1" s="27"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="31"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="30" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="H2" s="31"/>
+      <c r="H2" s="33"/>
       <c r="I2" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="K2" s="23"/>
-      <c r="L2" s="24"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="26"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -1259,7 +1292,7 @@
       <c r="K3" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="L3" s="27" t="s">
         <v>150</v>
       </c>
     </row>
@@ -1282,7 +1315,7 @@
       <c r="K4" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="L4" s="26"/>
+      <c r="L4" s="28"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
@@ -5110,7 +5143,7 @@
       <c r="K120" s="1">
         <v>-142.85</v>
       </c>
-      <c r="L120" s="33" t="s">
+      <c r="L120" s="22" t="s">
         <v>184</v>
       </c>
       <c r="M120" t="s">
@@ -5493,7 +5526,7 @@
       <c r="L130" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="M130" s="34" t="s">
+      <c r="M130" s="23" t="s">
         <v>179</v>
       </c>
     </row>
@@ -5531,7 +5564,7 @@
       <c r="L131" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="M131" s="34" t="s">
+      <c r="M131" s="23" t="s">
         <v>179</v>
       </c>
     </row>
@@ -5569,7 +5602,7 @@
       <c r="L132" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="M132" s="34" t="s">
+      <c r="M132" s="23" t="s">
         <v>179</v>
       </c>
     </row>
@@ -5607,8 +5640,305 @@
       <c r="L133" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="M133" s="34" t="s">
+      <c r="M133" s="23" t="s">
         <v>179</v>
+      </c>
+    </row>
+    <row r="135" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B135" s="1">
+        <v>1</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D135" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F135" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G135" s="1">
+        <v>25</v>
+      </c>
+      <c r="H135" s="1">
+        <v>-50</v>
+      </c>
+      <c r="I135" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="J135" s="1">
+        <v>0</v>
+      </c>
+      <c r="K135" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B136" s="1">
+        <v>1</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D136" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F136" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G136" s="1">
+        <v>100</v>
+      </c>
+      <c r="H136" s="1">
+        <v>100</v>
+      </c>
+      <c r="I136" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J136" s="1">
+        <v>100</v>
+      </c>
+      <c r="K136" s="1">
+        <v>100</v>
+      </c>
+      <c r="L136" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="137" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B137" s="1">
+        <v>1</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D137" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F137" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G137" s="1">
+        <v>0</v>
+      </c>
+      <c r="H137" s="1">
+        <v>0</v>
+      </c>
+      <c r="J137" s="1">
+        <v>0</v>
+      </c>
+      <c r="K137" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B138" s="1">
+        <v>2</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D138" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F138" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G138" s="1">
+        <v>0</v>
+      </c>
+      <c r="H138" s="1">
+        <v>0</v>
+      </c>
+      <c r="J138" s="1">
+        <v>-11.11</v>
+      </c>
+      <c r="K138" s="1">
+        <v>-400</v>
+      </c>
+      <c r="L138" s="9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="139" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B139" s="1">
+        <v>2</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D139" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F139" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="G139" s="1">
+        <v>66.66</v>
+      </c>
+      <c r="H139" s="1">
+        <v>-150</v>
+      </c>
+      <c r="I139" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="J139" s="1">
+        <v>66.66</v>
+      </c>
+      <c r="K139" s="1">
+        <v>-250</v>
+      </c>
+      <c r="L139" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="141" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B141" s="1">
+        <v>1</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D141" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F141" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="G141" s="1">
+        <v>100</v>
+      </c>
+      <c r="H141" s="1">
+        <v>100</v>
+      </c>
+      <c r="I141" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="J141" s="1">
+        <v>100</v>
+      </c>
+      <c r="K141" s="1">
+        <v>100</v>
+      </c>
+      <c r="L141" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="142" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B142" s="1">
+        <v>2</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D142" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F142" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="G142" s="1">
+        <v>0</v>
+      </c>
+      <c r="H142" s="1">
+        <v>0</v>
+      </c>
+      <c r="J142" s="1">
+        <v>100</v>
+      </c>
+      <c r="K142" s="1">
+        <v>100</v>
+      </c>
+      <c r="L142" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="143" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B143" s="1">
+        <v>2</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D143" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F143" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="G143" s="1">
+        <v>90</v>
+      </c>
+      <c r="H143" s="1">
+        <v>90</v>
+      </c>
+      <c r="I143" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="J143" s="1">
+        <v>100</v>
+      </c>
+      <c r="K143" s="1">
+        <v>100</v>
+      </c>
+      <c r="L143" s="9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="144" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B144" s="1">
+        <v>2</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D144" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F144" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="G144" s="1">
+        <v>90</v>
+      </c>
+      <c r="H144" s="1">
+        <v>90</v>
+      </c>
+      <c r="I144" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="J144" s="1">
+        <v>0</v>
+      </c>
+      <c r="K144" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>